<commit_message>
Adjusted numbering per fold for each method
</commit_message>
<xml_diff>
--- a/run_1/LinearRegression/LR_GLM/Tables/LR_performance_metrics_per_fold.xlsx
+++ b/run_1/LinearRegression/LR_GLM/Tables/LR_performance_metrics_per_fold.xlsx
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>